<commit_message>
added tests (news and claims pages) and auxiliary files
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -304,9 +304,6 @@
   </si>
   <si>
     <t>происходит переходна страницу "Заявки"</t>
-  </si>
-  <si>
-    <t>6.2. пролистывание страницы с блоками новостей</t>
   </si>
   <si>
     <t>список заявок сдвинется вверх</t>
@@ -788,6 +785,9 @@
   <si>
     <t>происходит переход на страницу блоков новостей, будут отображены не активные новости выбранной категории. Новость с внесенными изменениями появится в списке</t>
   </si>
+  <si>
+    <t>6.2. пролистывание страницы с блоками заявок</t>
+  </si>
 </sst>
 </file>
 
@@ -922,7 +922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -970,6 +970,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1255,8 +1258,8 @@
   </sheetPr>
   <dimension ref="A1:AD1038"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2345,7 +2348,7 @@
       <c r="AD28" s="10"/>
     </row>
     <row r="29" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="13">
+      <c r="A29" s="16">
         <v>9</v>
       </c>
       <c r="B29" s="13" t="s">
@@ -2389,7 +2392,7 @@
       <c r="AD29" s="6"/>
     </row>
     <row r="30" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -2425,7 +2428,7 @@
       <c r="AD30" s="6"/>
     </row>
     <row r="31" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="13">
+      <c r="A31" s="16">
         <v>10</v>
       </c>
       <c r="B31" s="13" t="s">
@@ -2469,7 +2472,7 @@
       <c r="AD31" s="6"/>
     </row>
     <row r="32" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -2505,7 +2508,7 @@
       <c r="AD32" s="6"/>
     </row>
     <row r="33" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
+      <c r="A33" s="16">
         <v>11</v>
       </c>
       <c r="B33" s="13" t="s">
@@ -2549,7 +2552,7 @@
       <c r="AD33" s="6"/>
     </row>
     <row r="34" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
@@ -2585,7 +2588,7 @@
       <c r="AD34" s="6"/>
     </row>
     <row r="35" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="13">
+      <c r="A35" s="16">
         <v>12</v>
       </c>
       <c r="B35" s="13" t="s">
@@ -2629,7 +2632,7 @@
       <c r="AD35" s="6"/>
     </row>
     <row r="36" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
@@ -2665,7 +2668,7 @@
       <c r="AD36" s="6"/>
     </row>
     <row r="37" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="13">
+      <c r="A37" s="16">
         <v>13</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -2709,7 +2712,7 @@
       <c r="AD37" s="6"/>
     </row>
     <row r="38" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
@@ -2745,7 +2748,7 @@
       <c r="AD38" s="6"/>
     </row>
     <row r="39" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="13">
+      <c r="A39" s="16">
         <v>14</v>
       </c>
       <c r="B39" s="13" t="s">
@@ -2789,7 +2792,7 @@
       <c r="AD39" s="6"/>
     </row>
     <row r="40" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15"/>
@@ -2825,7 +2828,7 @@
       <c r="AD40" s="6"/>
     </row>
     <row r="41" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="13">
+      <c r="A41" s="16">
         <v>15</v>
       </c>
       <c r="B41" s="13" t="s">
@@ -2869,7 +2872,7 @@
       <c r="AD41" s="6"/>
     </row>
     <row r="42" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15"/>
@@ -2905,7 +2908,7 @@
       <c r="AD42" s="6"/>
     </row>
     <row r="43" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="13">
+      <c r="A43" s="16">
         <v>16</v>
       </c>
       <c r="B43" s="13" t="s">
@@ -2949,7 +2952,7 @@
       <c r="AD43" s="6"/>
     </row>
     <row r="44" spans="1:30" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
@@ -2985,7 +2988,7 @@
       <c r="AD44" s="6"/>
     </row>
     <row r="45" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A45" s="13">
+      <c r="A45" s="16">
         <v>17</v>
       </c>
       <c r="B45" s="13" t="s">
@@ -3029,7 +3032,7 @@
       <c r="AD45" s="6"/>
     </row>
     <row r="46" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -3065,7 +3068,7 @@
       <c r="AD46" s="6"/>
     </row>
     <row r="47" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A47" s="13">
+      <c r="A47" s="16">
         <v>18</v>
       </c>
       <c r="B47" s="13" t="s">
@@ -3109,7 +3112,7 @@
       <c r="AD47" s="6"/>
     </row>
     <row r="48" spans="1:30" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
+      <c r="A48" s="17"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
@@ -3145,7 +3148,7 @@
       <c r="AD48" s="6"/>
     </row>
     <row r="49" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -3213,7 +3216,7 @@
       <c r="AD50" s="10"/>
     </row>
     <row r="51" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="13">
+      <c r="A51" s="16">
         <v>19</v>
       </c>
       <c r="B51" s="13" t="s">
@@ -3257,7 +3260,7 @@
       <c r="AD51" s="6"/>
     </row>
     <row r="52" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
+      <c r="A52" s="18"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
@@ -3293,7 +3296,7 @@
       <c r="AD52" s="6"/>
     </row>
     <row r="53" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="13">
+      <c r="A53" s="16">
         <v>20</v>
       </c>
       <c r="B53" s="13" t="s">
@@ -3337,7 +3340,7 @@
       <c r="AD53" s="6"/>
     </row>
     <row r="54" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="14"/>
+      <c r="A54" s="17"/>
       <c r="B54" s="14"/>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
@@ -3373,7 +3376,7 @@
       <c r="AD54" s="6"/>
     </row>
     <row r="55" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A55" s="15"/>
+      <c r="A55" s="18"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
@@ -3409,7 +3412,7 @@
       <c r="AD55" s="6"/>
     </row>
     <row r="56" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A56" s="13">
+      <c r="A56" s="16">
         <v>21</v>
       </c>
       <c r="B56" s="13" t="s">
@@ -3453,7 +3456,7 @@
       <c r="AD56" s="6"/>
     </row>
     <row r="57" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
+      <c r="A57" s="18"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
@@ -3521,7 +3524,7 @@
       <c r="AD58" s="10"/>
     </row>
     <row r="59" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="13">
+      <c r="A59" s="16">
         <v>22</v>
       </c>
       <c r="B59" s="13" t="s">
@@ -3565,7 +3568,7 @@
       <c r="AD59" s="6"/>
     </row>
     <row r="60" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+      <c r="A60" s="18"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
@@ -3633,7 +3636,7 @@
       <c r="AD61" s="10"/>
     </row>
     <row r="62" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A62" s="13">
+      <c r="A62" s="16">
         <v>23</v>
       </c>
       <c r="B62" s="13" t="s">
@@ -3677,7 +3680,7 @@
       <c r="AD62" s="6"/>
     </row>
     <row r="63" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
+      <c r="A63" s="18"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
@@ -3713,11 +3716,11 @@
       <c r="AD63" s="6"/>
     </row>
     <row r="64" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A64" s="13">
+      <c r="A64" s="16">
         <v>24</v>
       </c>
-      <c r="B64" s="13" t="s">
-        <v>95</v>
+      <c r="B64" s="19" t="s">
+        <v>255</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="13" t="s">
@@ -3730,7 +3733,7 @@
         <v>81</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
@@ -3757,7 +3760,7 @@
       <c r="AD64" s="6"/>
     </row>
     <row r="65" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
+      <c r="A65" s="18"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
       <c r="D65" s="15"/>
@@ -3766,7 +3769,7 @@
         <v>83</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
@@ -3793,11 +3796,11 @@
       <c r="AD65" s="6"/>
     </row>
     <row r="66" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A66" s="13">
+      <c r="A66" s="16">
         <v>25</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="13" t="s">
@@ -3807,10 +3810,10 @@
         <v>48</v>
       </c>
       <c r="F66" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G66" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
@@ -3837,16 +3840,16 @@
       <c r="AD66" s="6"/>
     </row>
     <row r="67" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
+      <c r="A67" s="17"/>
       <c r="B67" s="14"/>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G67" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
@@ -3873,16 +3876,16 @@
       <c r="AD67" s="6"/>
     </row>
     <row r="68" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
+      <c r="A68" s="17"/>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G68" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
@@ -3909,16 +3912,16 @@
       <c r="AD68" s="6"/>
     </row>
     <row r="69" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
+      <c r="A69" s="17"/>
       <c r="B69" s="14"/>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G69" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -3945,16 +3948,16 @@
       <c r="AD69" s="6"/>
     </row>
     <row r="70" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
+      <c r="A70" s="17"/>
       <c r="B70" s="14"/>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G70" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="G70" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
@@ -3981,16 +3984,16 @@
       <c r="AD70" s="6"/>
     </row>
     <row r="71" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
+      <c r="A71" s="18"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
       <c r="E71" s="15"/>
       <c r="F71" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G71" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="H71" s="6"/>
       <c r="I71" s="6"/>
@@ -4017,11 +4020,11 @@
       <c r="AD71" s="6"/>
     </row>
     <row r="72" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A72" s="13">
+      <c r="A72" s="16">
         <v>26</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13" t="s">
@@ -4031,10 +4034,10 @@
         <v>48</v>
       </c>
       <c r="F72" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G72" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="G72" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
@@ -4061,13 +4064,13 @@
       <c r="AD72" s="6"/>
     </row>
     <row r="73" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
+      <c r="A73" s="17"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G73" s="7"/>
       <c r="H73" s="6"/>
@@ -4095,16 +4098,16 @@
       <c r="AD73" s="6"/>
     </row>
     <row r="74" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
+      <c r="A74" s="17"/>
       <c r="B74" s="14"/>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G74" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
@@ -4131,16 +4134,16 @@
       <c r="AD74" s="6"/>
     </row>
     <row r="75" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A75" s="14"/>
+      <c r="A75" s="17"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G75" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
@@ -4167,16 +4170,16 @@
       <c r="AD75" s="6"/>
     </row>
     <row r="76" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
+      <c r="A76" s="17"/>
       <c r="B76" s="14"/>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G76" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
@@ -4203,16 +4206,16 @@
       <c r="AD76" s="6"/>
     </row>
     <row r="77" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A77" s="15"/>
+      <c r="A77" s="18"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
       <c r="D77" s="15"/>
       <c r="E77" s="15"/>
       <c r="F77" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
@@ -4239,11 +4242,11 @@
       <c r="AD77" s="6"/>
     </row>
     <row r="78" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A78" s="13">
+      <c r="A78" s="16">
         <v>27</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13" t="s">
@@ -4253,10 +4256,10 @@
         <v>48</v>
       </c>
       <c r="F78" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G78" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
@@ -4283,16 +4286,16 @@
       <c r="AD78" s="6"/>
     </row>
     <row r="79" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
+      <c r="A79" s="17"/>
       <c r="B79" s="14"/>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G79" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="G79" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
@@ -4319,16 +4322,16 @@
       <c r="AD79" s="6"/>
     </row>
     <row r="80" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
+      <c r="A80" s="17"/>
       <c r="B80" s="14"/>
       <c r="C80" s="14"/>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="G80" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
@@ -4355,13 +4358,13 @@
       <c r="AD80" s="6"/>
     </row>
     <row r="81" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
+      <c r="A81" s="17"/>
       <c r="B81" s="14"/>
       <c r="C81" s="14"/>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G81" s="7"/>
       <c r="H81" s="6"/>
@@ -4389,16 +4392,16 @@
       <c r="AD81" s="6"/>
     </row>
     <row r="82" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A82" s="14"/>
+      <c r="A82" s="17"/>
       <c r="B82" s="14"/>
       <c r="C82" s="14"/>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G82" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
@@ -4425,16 +4428,16 @@
       <c r="AD82" s="6"/>
     </row>
     <row r="83" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A83" s="15"/>
+      <c r="A83" s="18"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
       <c r="F83" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
@@ -4461,11 +4464,11 @@
       <c r="AD83" s="6"/>
     </row>
     <row r="84" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A84" s="13">
+      <c r="A84" s="16">
         <v>28</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C84" s="13"/>
       <c r="D84" s="13" t="s">
@@ -4475,10 +4478,10 @@
         <v>48</v>
       </c>
       <c r="F84" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G84" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>100</v>
       </c>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
@@ -4505,16 +4508,16 @@
       <c r="AD84" s="6"/>
     </row>
     <row r="85" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="14"/>
+      <c r="A85" s="17"/>
       <c r="B85" s="14"/>
       <c r="C85" s="14"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G85" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
@@ -4541,13 +4544,13 @@
       <c r="AD85" s="6"/>
     </row>
     <row r="86" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="14"/>
+      <c r="A86" s="17"/>
       <c r="B86" s="14"/>
       <c r="C86" s="14"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G86" s="7"/>
       <c r="H86" s="6"/>
@@ -4575,16 +4578,16 @@
       <c r="AD86" s="6"/>
     </row>
     <row r="87" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="14"/>
+      <c r="A87" s="17"/>
       <c r="B87" s="14"/>
       <c r="C87" s="14"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="G87" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="H87" s="6"/>
       <c r="I87" s="6"/>
@@ -4611,16 +4614,16 @@
       <c r="AD87" s="6"/>
     </row>
     <row r="88" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="14"/>
+      <c r="A88" s="17"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G88" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="H88" s="6"/>
       <c r="I88" s="6"/>
@@ -4647,16 +4650,16 @@
       <c r="AD88" s="6"/>
     </row>
     <row r="89" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="15"/>
+      <c r="A89" s="18"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
       <c r="D89" s="15"/>
       <c r="E89" s="15"/>
       <c r="F89" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G89" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G89" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="H89" s="6"/>
       <c r="I89" s="6"/>
@@ -4683,11 +4686,11 @@
       <c r="AD89" s="6"/>
     </row>
     <row r="90" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="13">
+      <c r="A90" s="16">
         <v>29</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C90" s="13"/>
       <c r="D90" s="13" t="s">
@@ -4727,16 +4730,16 @@
       <c r="AD90" s="6"/>
     </row>
     <row r="91" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
+      <c r="A91" s="17"/>
       <c r="B91" s="14"/>
       <c r="C91" s="14"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G91" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="H91" s="6"/>
       <c r="I91" s="6"/>
@@ -4763,16 +4766,16 @@
       <c r="AD91" s="6"/>
     </row>
     <row r="92" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A92" s="14"/>
+      <c r="A92" s="17"/>
       <c r="B92" s="14"/>
       <c r="C92" s="14"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G92" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>122</v>
       </c>
       <c r="H92" s="6"/>
       <c r="I92" s="6"/>
@@ -4799,16 +4802,16 @@
       <c r="AD92" s="6"/>
     </row>
     <row r="93" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="15"/>
+      <c r="A93" s="18"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
       <c r="F93" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G93" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G93" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="H93" s="6"/>
       <c r="I93" s="6"/>
@@ -4835,11 +4838,11 @@
       <c r="AD93" s="6"/>
     </row>
     <row r="94" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="13">
+      <c r="A94" s="16">
         <v>30</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C94" s="13"/>
       <c r="D94" s="13" t="s">
@@ -4879,16 +4882,16 @@
       <c r="AD94" s="6"/>
     </row>
     <row r="95" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A95" s="14"/>
+      <c r="A95" s="17"/>
       <c r="B95" s="14"/>
       <c r="C95" s="14"/>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G95" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="G95" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="H95" s="6"/>
       <c r="I95" s="6"/>
@@ -4915,16 +4918,16 @@
       <c r="AD95" s="6"/>
     </row>
     <row r="96" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="14"/>
+      <c r="A96" s="17"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G96" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="H96" s="6"/>
       <c r="I96" s="6"/>
@@ -4951,16 +4954,16 @@
       <c r="AD96" s="6"/>
     </row>
     <row r="97" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="14"/>
+      <c r="A97" s="17"/>
       <c r="B97" s="14"/>
       <c r="C97" s="14"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G97" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="G97" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="H97" s="6"/>
       <c r="I97" s="6"/>
@@ -4987,16 +4990,16 @@
       <c r="AD97" s="6"/>
     </row>
     <row r="98" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A98" s="14"/>
+      <c r="A98" s="17"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G98" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="G98" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="H98" s="6"/>
       <c r="I98" s="6"/>
@@ -5023,16 +5026,16 @@
       <c r="AD98" s="6"/>
     </row>
     <row r="99" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A99" s="15"/>
+      <c r="A99" s="18"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
       <c r="F99" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G99" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="G99" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="H99" s="6"/>
       <c r="I99" s="6"/>
@@ -5059,11 +5062,11 @@
       <c r="AD99" s="6"/>
     </row>
     <row r="100" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A100" s="13">
+      <c r="A100" s="16">
         <v>31</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C100" s="13"/>
       <c r="D100" s="13" t="s">
@@ -5103,16 +5106,16 @@
       <c r="AD100" s="6"/>
     </row>
     <row r="101" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A101" s="14"/>
+      <c r="A101" s="17"/>
       <c r="B101" s="14"/>
       <c r="C101" s="14"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
       <c r="F101" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G101" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="G101" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="H101" s="6"/>
       <c r="I101" s="6"/>
@@ -5139,13 +5142,13 @@
       <c r="AD101" s="6"/>
     </row>
     <row r="102" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A102" s="14"/>
+      <c r="A102" s="17"/>
       <c r="B102" s="14"/>
       <c r="C102" s="14"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G102" s="7"/>
       <c r="H102" s="6"/>
@@ -5173,16 +5176,16 @@
       <c r="AD102" s="6"/>
     </row>
     <row r="103" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="14"/>
+      <c r="A103" s="17"/>
       <c r="B103" s="14"/>
       <c r="C103" s="14"/>
       <c r="D103" s="14"/>
       <c r="E103" s="14"/>
       <c r="F103" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G103" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="G103" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="H103" s="6"/>
       <c r="I103" s="6"/>
@@ -5209,16 +5212,16 @@
       <c r="AD103" s="6"/>
     </row>
     <row r="104" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A104" s="14"/>
+      <c r="A104" s="17"/>
       <c r="B104" s="14"/>
       <c r="C104" s="14"/>
       <c r="D104" s="14"/>
       <c r="E104" s="14"/>
       <c r="F104" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G104" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="G104" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="H104" s="6"/>
       <c r="I104" s="6"/>
@@ -5245,16 +5248,16 @@
       <c r="AD104" s="6"/>
     </row>
     <row r="105" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A105" s="15"/>
+      <c r="A105" s="18"/>
       <c r="B105" s="15"/>
       <c r="C105" s="15"/>
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
       <c r="F105" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H105" s="6"/>
       <c r="I105" s="6"/>
@@ -5281,11 +5284,11 @@
       <c r="AD105" s="6"/>
     </row>
     <row r="106" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A106" s="13">
+      <c r="A106" s="16">
         <v>32</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="13" t="s">
@@ -5325,16 +5328,16 @@
       <c r="AD106" s="6"/>
     </row>
     <row r="107" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A107" s="14"/>
+      <c r="A107" s="17"/>
       <c r="B107" s="14"/>
       <c r="C107" s="14"/>
       <c r="D107" s="14"/>
       <c r="E107" s="14"/>
       <c r="F107" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G107" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="G107" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="H107" s="6"/>
       <c r="I107" s="6"/>
@@ -5361,16 +5364,16 @@
       <c r="AD107" s="6"/>
     </row>
     <row r="108" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A108" s="14"/>
+      <c r="A108" s="17"/>
       <c r="B108" s="14"/>
       <c r="C108" s="14"/>
       <c r="D108" s="14"/>
       <c r="E108" s="14"/>
       <c r="F108" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G108" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="G108" s="7" t="s">
-        <v>127</v>
       </c>
       <c r="H108" s="6"/>
       <c r="I108" s="6"/>
@@ -5397,13 +5400,13 @@
       <c r="AD108" s="6"/>
     </row>
     <row r="109" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A109" s="14"/>
+      <c r="A109" s="17"/>
       <c r="B109" s="14"/>
       <c r="C109" s="14"/>
       <c r="D109" s="14"/>
       <c r="E109" s="14"/>
       <c r="F109" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G109" s="7"/>
       <c r="H109" s="6"/>
@@ -5431,16 +5434,16 @@
       <c r="AD109" s="6"/>
     </row>
     <row r="110" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A110" s="14"/>
+      <c r="A110" s="17"/>
       <c r="B110" s="14"/>
       <c r="C110" s="14"/>
       <c r="D110" s="14"/>
       <c r="E110" s="14"/>
       <c r="F110" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G110" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="G110" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="H110" s="6"/>
       <c r="I110" s="6"/>
@@ -5467,16 +5470,16 @@
       <c r="AD110" s="6"/>
     </row>
     <row r="111" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A111" s="15"/>
+      <c r="A111" s="18"/>
       <c r="B111" s="15"/>
       <c r="C111" s="15"/>
       <c r="D111" s="15"/>
       <c r="E111" s="15"/>
       <c r="F111" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G111" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H111" s="6"/>
       <c r="I111" s="6"/>
@@ -5503,11 +5506,11 @@
       <c r="AD111" s="6"/>
     </row>
     <row r="112" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A112" s="13">
+      <c r="A112" s="16">
         <v>33</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C112" s="13"/>
       <c r="D112" s="13" t="s">
@@ -5517,10 +5520,10 @@
         <v>48</v>
       </c>
       <c r="F112" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G112" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="G112" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="H112" s="6"/>
       <c r="I112" s="6"/>
@@ -5547,16 +5550,16 @@
       <c r="AD112" s="6"/>
     </row>
     <row r="113" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A113" s="14"/>
+      <c r="A113" s="17"/>
       <c r="B113" s="14"/>
       <c r="C113" s="14"/>
       <c r="D113" s="14"/>
       <c r="E113" s="14"/>
       <c r="F113" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="G113" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="G113" s="7" t="s">
-        <v>139</v>
       </c>
       <c r="H113" s="6"/>
       <c r="I113" s="6"/>
@@ -5583,16 +5586,16 @@
       <c r="AD113" s="6"/>
     </row>
     <row r="114" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A114" s="15"/>
+      <c r="A114" s="18"/>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
       <c r="D114" s="15"/>
       <c r="E114" s="15"/>
       <c r="F114" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G114" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="G114" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="H114" s="6"/>
       <c r="I114" s="6"/>
@@ -5619,11 +5622,11 @@
       <c r="AD114" s="6"/>
     </row>
     <row r="115" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A115" s="13">
+      <c r="A115" s="16">
         <v>34</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C115" s="13"/>
       <c r="D115" s="13" t="s">
@@ -5633,10 +5636,10 @@
         <v>48</v>
       </c>
       <c r="F115" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G115" s="7" t="s">
         <v>136</v>
-      </c>
-      <c r="G115" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="H115" s="6"/>
       <c r="I115" s="6"/>
@@ -5663,16 +5666,16 @@
       <c r="AD115" s="6"/>
     </row>
     <row r="116" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A116" s="14"/>
+      <c r="A116" s="17"/>
       <c r="B116" s="14"/>
       <c r="C116" s="14"/>
       <c r="D116" s="14"/>
       <c r="E116" s="14"/>
       <c r="F116" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G116" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="G116" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="H116" s="6"/>
       <c r="I116" s="6"/>
@@ -5699,16 +5702,16 @@
       <c r="AD116" s="6"/>
     </row>
     <row r="117" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A117" s="14"/>
+      <c r="A117" s="17"/>
       <c r="B117" s="14"/>
       <c r="C117" s="14"/>
       <c r="D117" s="14"/>
       <c r="E117" s="14"/>
       <c r="F117" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G117" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H117" s="6"/>
       <c r="I117" s="6"/>
@@ -5735,16 +5738,16 @@
       <c r="AD117" s="6"/>
     </row>
     <row r="118" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A118" s="15"/>
+      <c r="A118" s="18"/>
       <c r="B118" s="15"/>
       <c r="C118" s="15"/>
       <c r="D118" s="15"/>
       <c r="E118" s="15"/>
       <c r="F118" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G118" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="G118" s="7" t="s">
-        <v>147</v>
       </c>
       <c r="H118" s="11"/>
       <c r="I118" s="6"/>
@@ -5771,11 +5774,11 @@
       <c r="AD118" s="6"/>
     </row>
     <row r="119" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A119" s="13">
+      <c r="A119" s="16">
         <v>35</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C119" s="13"/>
       <c r="D119" s="13" t="s">
@@ -5815,16 +5818,16 @@
       <c r="AD119" s="6"/>
     </row>
     <row r="120" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A120" s="14"/>
+      <c r="A120" s="17"/>
       <c r="B120" s="14"/>
       <c r="C120" s="14"/>
       <c r="D120" s="14"/>
       <c r="E120" s="14"/>
       <c r="F120" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G120" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="G120" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="H120" s="6"/>
       <c r="I120" s="6"/>
@@ -5851,16 +5854,16 @@
       <c r="AD120" s="6"/>
     </row>
     <row r="121" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A121" s="14"/>
+      <c r="A121" s="17"/>
       <c r="B121" s="14"/>
       <c r="C121" s="14"/>
       <c r="D121" s="14"/>
       <c r="E121" s="14"/>
       <c r="F121" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G121" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="G121" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="H121" s="6"/>
       <c r="I121" s="6"/>
@@ -5887,16 +5890,16 @@
       <c r="AD121" s="6"/>
     </row>
     <row r="122" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A122" s="15"/>
+      <c r="A122" s="18"/>
       <c r="B122" s="15"/>
       <c r="C122" s="15"/>
       <c r="D122" s="15"/>
       <c r="E122" s="15"/>
       <c r="F122" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G122" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="G122" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="H122" s="6"/>
       <c r="I122" s="6"/>
@@ -5923,11 +5926,11 @@
       <c r="AD122" s="6"/>
     </row>
     <row r="123" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A123" s="13">
+      <c r="A123" s="16">
         <v>36</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="13" t="s">
@@ -5967,16 +5970,16 @@
       <c r="AD123" s="6"/>
     </row>
     <row r="124" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A124" s="14"/>
+      <c r="A124" s="17"/>
       <c r="B124" s="14"/>
       <c r="C124" s="14"/>
       <c r="D124" s="14"/>
       <c r="E124" s="14"/>
       <c r="F124" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G124" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="G124" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="H124" s="6"/>
       <c r="I124" s="6"/>
@@ -6003,13 +6006,13 @@
       <c r="AD124" s="6"/>
     </row>
     <row r="125" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A125" s="14"/>
+      <c r="A125" s="17"/>
       <c r="B125" s="14"/>
       <c r="C125" s="14"/>
       <c r="D125" s="14"/>
       <c r="E125" s="14"/>
       <c r="F125" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G125" s="7"/>
       <c r="H125" s="6"/>
@@ -6037,16 +6040,16 @@
       <c r="AD125" s="6"/>
     </row>
     <row r="126" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A126" s="15"/>
+      <c r="A126" s="18"/>
       <c r="B126" s="15"/>
       <c r="C126" s="15"/>
       <c r="D126" s="15"/>
       <c r="E126" s="15"/>
       <c r="F126" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="6"/>
@@ -6073,11 +6076,11 @@
       <c r="AD126" s="6"/>
     </row>
     <row r="127" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A127" s="13">
+      <c r="A127" s="16">
         <v>37</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C127" s="13"/>
       <c r="D127" s="13" t="s">
@@ -6117,16 +6120,16 @@
       <c r="AD127" s="6"/>
     </row>
     <row r="128" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A128" s="14"/>
+      <c r="A128" s="17"/>
       <c r="B128" s="14"/>
       <c r="C128" s="14"/>
       <c r="D128" s="14"/>
       <c r="E128" s="14"/>
       <c r="F128" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G128" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="G128" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="H128" s="6"/>
       <c r="I128" s="6"/>
@@ -6153,16 +6156,16 @@
       <c r="AD128" s="6"/>
     </row>
     <row r="129" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A129" s="14"/>
+      <c r="A129" s="17"/>
       <c r="B129" s="14"/>
       <c r="C129" s="14"/>
       <c r="D129" s="14"/>
       <c r="E129" s="14"/>
       <c r="F129" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G129" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="G129" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="H129" s="6"/>
       <c r="I129" s="6"/>
@@ -6189,16 +6192,16 @@
       <c r="AD129" s="6"/>
     </row>
     <row r="130" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A130" s="14"/>
+      <c r="A130" s="17"/>
       <c r="B130" s="14"/>
       <c r="C130" s="14"/>
       <c r="D130" s="14"/>
       <c r="E130" s="14"/>
       <c r="F130" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G130" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="G130" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="H130" s="6"/>
       <c r="I130" s="6"/>
@@ -6225,16 +6228,16 @@
       <c r="AD130" s="6"/>
     </row>
     <row r="131" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A131" s="14"/>
+      <c r="A131" s="17"/>
       <c r="B131" s="14"/>
       <c r="C131" s="14"/>
       <c r="D131" s="14"/>
       <c r="E131" s="14"/>
       <c r="F131" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G131" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="G131" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="H131" s="6"/>
       <c r="I131" s="6"/>
@@ -6261,16 +6264,16 @@
       <c r="AD131" s="6"/>
     </row>
     <row r="132" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A132" s="14"/>
+      <c r="A132" s="17"/>
       <c r="B132" s="14"/>
       <c r="C132" s="14"/>
       <c r="D132" s="14"/>
       <c r="E132" s="14"/>
       <c r="F132" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G132" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="G132" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="H132" s="6"/>
       <c r="I132" s="6"/>
@@ -6297,16 +6300,16 @@
       <c r="AD132" s="6"/>
     </row>
     <row r="133" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A133" s="15"/>
+      <c r="A133" s="18"/>
       <c r="B133" s="15"/>
       <c r="C133" s="15"/>
       <c r="D133" s="15"/>
       <c r="E133" s="15"/>
       <c r="F133" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G133" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="G133" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="H133" s="6"/>
       <c r="I133" s="6"/>
@@ -6333,11 +6336,11 @@
       <c r="AD133" s="6"/>
     </row>
     <row r="134" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A134" s="13">
+      <c r="A134" s="16">
         <v>38</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C134" s="13"/>
       <c r="D134" s="13" t="s">
@@ -6377,16 +6380,16 @@
       <c r="AD134" s="6"/>
     </row>
     <row r="135" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A135" s="14"/>
+      <c r="A135" s="17"/>
       <c r="B135" s="14"/>
       <c r="C135" s="14"/>
       <c r="D135" s="14"/>
       <c r="E135" s="14"/>
       <c r="F135" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G135" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="G135" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="H135" s="6"/>
       <c r="I135" s="6"/>
@@ -6413,16 +6416,16 @@
       <c r="AD135" s="6"/>
     </row>
     <row r="136" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A136" s="14"/>
+      <c r="A136" s="17"/>
       <c r="B136" s="14"/>
       <c r="C136" s="14"/>
       <c r="D136" s="14"/>
       <c r="E136" s="14"/>
       <c r="F136" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="G136" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="G136" s="7" t="s">
-        <v>152</v>
       </c>
       <c r="H136" s="6"/>
       <c r="I136" s="6"/>
@@ -6449,16 +6452,16 @@
       <c r="AD136" s="6"/>
     </row>
     <row r="137" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A137" s="14"/>
+      <c r="A137" s="17"/>
       <c r="B137" s="14"/>
       <c r="C137" s="14"/>
       <c r="D137" s="14"/>
       <c r="E137" s="14"/>
       <c r="F137" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G137" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="G137" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="H137" s="6"/>
       <c r="I137" s="6"/>
@@ -6485,16 +6488,16 @@
       <c r="AD137" s="6"/>
     </row>
     <row r="138" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A138" s="14"/>
+      <c r="A138" s="17"/>
       <c r="B138" s="14"/>
       <c r="C138" s="14"/>
       <c r="D138" s="14"/>
       <c r="E138" s="14"/>
       <c r="F138" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="G138" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="G138" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="H138" s="6"/>
       <c r="I138" s="6"/>
@@ -6521,13 +6524,13 @@
       <c r="AD138" s="6"/>
     </row>
     <row r="139" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A139" s="14"/>
+      <c r="A139" s="17"/>
       <c r="B139" s="14"/>
       <c r="C139" s="14"/>
       <c r="D139" s="14"/>
       <c r="E139" s="14"/>
       <c r="F139" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G139" s="7"/>
       <c r="H139" s="6"/>
@@ -6555,16 +6558,16 @@
       <c r="AD139" s="6"/>
     </row>
     <row r="140" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A140" s="15"/>
+      <c r="A140" s="18"/>
       <c r="B140" s="15"/>
       <c r="C140" s="15"/>
       <c r="D140" s="15"/>
       <c r="E140" s="15"/>
       <c r="F140" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H140" s="6"/>
       <c r="I140" s="6"/>
@@ -6627,7 +6630,7 @@
         <v>39</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C142" s="13"/>
       <c r="D142" s="13" t="s">
@@ -6637,10 +6640,10 @@
         <v>55</v>
       </c>
       <c r="F142" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G142" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="G142" s="7" t="s">
-        <v>169</v>
       </c>
       <c r="H142" s="6"/>
       <c r="I142" s="6"/>
@@ -6673,7 +6676,7 @@
       <c r="D143" s="15"/>
       <c r="E143" s="15"/>
       <c r="F143" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G143" s="7" t="s">
         <v>78</v>
@@ -6707,7 +6710,7 @@
         <v>40</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C144" s="13"/>
       <c r="D144" s="13" t="s">
@@ -6720,7 +6723,7 @@
         <v>81</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H144" s="6"/>
       <c r="I144" s="6"/>
@@ -6756,7 +6759,7 @@
         <v>83</v>
       </c>
       <c r="G145" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H145" s="6"/>
       <c r="I145" s="6"/>
@@ -6787,7 +6790,7 @@
         <v>41</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C146" s="13"/>
       <c r="D146" s="13" t="s">
@@ -6797,10 +6800,10 @@
         <v>55</v>
       </c>
       <c r="F146" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G146" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="G146" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="H146" s="6"/>
       <c r="I146" s="6"/>
@@ -6833,10 +6836,10 @@
       <c r="D147" s="15"/>
       <c r="E147" s="15"/>
       <c r="F147" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="G147" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="G147" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="H147" s="6"/>
       <c r="I147" s="6"/>
@@ -6867,7 +6870,7 @@
         <v>42</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C148" s="13"/>
       <c r="D148" s="13" t="s">
@@ -6877,10 +6880,10 @@
         <v>55</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G148" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H148" s="6"/>
       <c r="I148" s="6"/>
@@ -6913,10 +6916,10 @@
       <c r="D149" s="14"/>
       <c r="E149" s="14"/>
       <c r="F149" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G149" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="G149" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="H149" s="6"/>
       <c r="I149" s="6"/>
@@ -6949,10 +6952,10 @@
       <c r="D150" s="15"/>
       <c r="E150" s="15"/>
       <c r="F150" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="G150" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="G150" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="H150" s="6"/>
       <c r="I150" s="6"/>
@@ -6983,7 +6986,7 @@
         <v>43</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C151" s="13"/>
       <c r="D151" s="13" t="s">
@@ -6993,10 +6996,10 @@
         <v>55</v>
       </c>
       <c r="F151" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H151" s="6"/>
       <c r="I151" s="6"/>
@@ -7029,10 +7032,10 @@
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
       <c r="F152" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G152" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="G152" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="H152" s="6"/>
       <c r="I152" s="6"/>
@@ -7065,10 +7068,10 @@
       <c r="D153" s="15"/>
       <c r="E153" s="15"/>
       <c r="F153" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H153" s="6"/>
       <c r="I153" s="6"/>
@@ -7099,7 +7102,7 @@
         <v>44</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C154" s="13"/>
       <c r="D154" s="13" t="s">
@@ -7109,10 +7112,10 @@
         <v>55</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H154" s="6"/>
       <c r="I154" s="6"/>
@@ -7145,10 +7148,10 @@
       <c r="D155" s="14"/>
       <c r="E155" s="14"/>
       <c r="F155" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="G155" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="G155" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="H155" s="6"/>
       <c r="I155" s="6"/>
@@ -7181,10 +7184,10 @@
       <c r="D156" s="14"/>
       <c r="E156" s="14"/>
       <c r="F156" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G156" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H156" s="6"/>
       <c r="I156" s="6"/>
@@ -7217,10 +7220,10 @@
       <c r="D157" s="15"/>
       <c r="E157" s="15"/>
       <c r="F157" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="G157" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="G157" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="H157" s="6"/>
       <c r="I157" s="6"/>
@@ -7251,7 +7254,7 @@
         <v>45</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C158" s="13"/>
       <c r="D158" s="13" t="s">
@@ -7261,10 +7264,10 @@
         <v>55</v>
       </c>
       <c r="F158" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G158" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G158" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H158" s="6"/>
       <c r="I158" s="6"/>
@@ -7297,10 +7300,10 @@
       <c r="D159" s="14"/>
       <c r="E159" s="14"/>
       <c r="F159" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G159" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H159" s="6"/>
       <c r="I159" s="6"/>
@@ -7333,10 +7336,10 @@
       <c r="D160" s="15"/>
       <c r="E160" s="15"/>
       <c r="F160" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G160" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H160" s="6"/>
       <c r="I160" s="6"/>
@@ -7367,7 +7370,7 @@
         <v>46</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C161" s="13"/>
       <c r="D161" s="13" t="s">
@@ -7377,10 +7380,10 @@
         <v>55</v>
       </c>
       <c r="F161" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G161" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G161" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H161" s="6"/>
       <c r="I161" s="6"/>
@@ -7413,10 +7416,10 @@
       <c r="D162" s="14"/>
       <c r="E162" s="14"/>
       <c r="F162" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G162" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H162" s="6"/>
       <c r="I162" s="6"/>
@@ -7449,10 +7452,10 @@
       <c r="D163" s="14"/>
       <c r="E163" s="14"/>
       <c r="F163" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G163" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H163" s="6"/>
       <c r="I163" s="6"/>
@@ -7485,10 +7488,10 @@
       <c r="D164" s="14"/>
       <c r="E164" s="14"/>
       <c r="F164" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G164" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H164" s="6"/>
       <c r="I164" s="6"/>
@@ -7521,10 +7524,10 @@
       <c r="D165" s="14"/>
       <c r="E165" s="14"/>
       <c r="F165" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G165" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="G165" s="7" t="s">
-        <v>203</v>
       </c>
       <c r="H165" s="6"/>
       <c r="I165" s="6"/>
@@ -7557,10 +7560,10 @@
       <c r="D166" s="15"/>
       <c r="E166" s="15"/>
       <c r="F166" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G166" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H166" s="6"/>
       <c r="I166" s="6"/>
@@ -7591,7 +7594,7 @@
         <v>47</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C167" s="13"/>
       <c r="D167" s="13" t="s">
@@ -7601,10 +7604,10 @@
         <v>55</v>
       </c>
       <c r="F167" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G167" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G167" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H167" s="6"/>
       <c r="I167" s="6"/>
@@ -7637,10 +7640,10 @@
       <c r="D168" s="14"/>
       <c r="E168" s="14"/>
       <c r="F168" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G168" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="G168" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="H168" s="6"/>
       <c r="I168" s="6"/>
@@ -7673,10 +7676,10 @@
       <c r="D169" s="14"/>
       <c r="E169" s="14"/>
       <c r="F169" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G169" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="G169" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="H169" s="6"/>
       <c r="I169" s="6"/>
@@ -7709,10 +7712,10 @@
       <c r="D170" s="14"/>
       <c r="E170" s="14"/>
       <c r="F170" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G170" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="G170" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="H170" s="6"/>
       <c r="I170" s="6"/>
@@ -7745,10 +7748,10 @@
       <c r="D171" s="14"/>
       <c r="E171" s="14"/>
       <c r="F171" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G171" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H171" s="6"/>
       <c r="I171" s="6"/>
@@ -7781,10 +7784,10 @@
       <c r="D172" s="14"/>
       <c r="E172" s="14"/>
       <c r="F172" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G172" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="G172" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="H172" s="6"/>
       <c r="I172" s="6"/>
@@ -7817,10 +7820,10 @@
       <c r="D173" s="15"/>
       <c r="E173" s="15"/>
       <c r="F173" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G173" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="G173" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="H173" s="6"/>
       <c r="I173" s="6"/>
@@ -7851,7 +7854,7 @@
         <v>48</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C174" s="13"/>
       <c r="D174" s="13" t="s">
@@ -7861,10 +7864,10 @@
         <v>55</v>
       </c>
       <c r="F174" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G174" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G174" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H174" s="6"/>
       <c r="I174" s="6"/>
@@ -7897,10 +7900,10 @@
       <c r="D175" s="14"/>
       <c r="E175" s="14"/>
       <c r="F175" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G175" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="G175" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="H175" s="6"/>
       <c r="I175" s="6"/>
@@ -7933,10 +7936,10 @@
       <c r="D176" s="14"/>
       <c r="E176" s="14"/>
       <c r="F176" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G176" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="G176" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="H176" s="6"/>
       <c r="I176" s="6"/>
@@ -7969,7 +7972,7 @@
       <c r="D177" s="14"/>
       <c r="E177" s="14"/>
       <c r="F177" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G177" s="7"/>
       <c r="H177" s="6"/>
@@ -8003,10 +8006,10 @@
       <c r="D178" s="14"/>
       <c r="E178" s="14"/>
       <c r="F178" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G178" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H178" s="6"/>
       <c r="I178" s="6"/>
@@ -8039,10 +8042,10 @@
       <c r="D179" s="14"/>
       <c r="E179" s="14"/>
       <c r="F179" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G179" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="G179" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="H179" s="6"/>
       <c r="I179" s="6"/>
@@ -8075,10 +8078,10 @@
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
       <c r="F180" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G180" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H180" s="6"/>
       <c r="I180" s="6"/>
@@ -8109,7 +8112,7 @@
         <v>49</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C181" s="13"/>
       <c r="D181" s="13" t="s">
@@ -8119,10 +8122,10 @@
         <v>55</v>
       </c>
       <c r="F181" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G181" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G181" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H181" s="6"/>
       <c r="I181" s="6"/>
@@ -8155,10 +8158,10 @@
       <c r="D182" s="14"/>
       <c r="E182" s="14"/>
       <c r="F182" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G182" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="G182" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="H182" s="6"/>
       <c r="I182" s="6"/>
@@ -8191,10 +8194,10 @@
       <c r="D183" s="14"/>
       <c r="E183" s="14"/>
       <c r="F183" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G183" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H183" s="6"/>
       <c r="I183" s="6"/>
@@ -8227,7 +8230,7 @@
       <c r="D184" s="14"/>
       <c r="E184" s="14"/>
       <c r="F184" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G184" s="7"/>
       <c r="H184" s="6"/>
@@ -8261,10 +8264,10 @@
       <c r="D185" s="14"/>
       <c r="E185" s="14"/>
       <c r="F185" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G185" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H185" s="6"/>
       <c r="I185" s="6"/>
@@ -8297,10 +8300,10 @@
       <c r="D186" s="14"/>
       <c r="E186" s="14"/>
       <c r="F186" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G186" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="G186" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="H186" s="6"/>
       <c r="I186" s="6"/>
@@ -8333,10 +8336,10 @@
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
       <c r="F187" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G187" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H187" s="6"/>
       <c r="I187" s="6"/>
@@ -8367,7 +8370,7 @@
         <v>50</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13" t="s">
@@ -8377,10 +8380,10 @@
         <v>55</v>
       </c>
       <c r="F188" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G188" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G188" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H188" s="6"/>
       <c r="I188" s="6"/>
@@ -8413,10 +8416,10 @@
       <c r="D189" s="14"/>
       <c r="E189" s="14"/>
       <c r="F189" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G189" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="G189" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="H189" s="6"/>
       <c r="I189" s="6"/>
@@ -8449,10 +8452,10 @@
       <c r="D190" s="14"/>
       <c r="E190" s="14"/>
       <c r="F190" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G190" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="G190" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="H190" s="6"/>
       <c r="I190" s="6"/>
@@ -8485,10 +8488,10 @@
       <c r="D191" s="14"/>
       <c r="E191" s="14"/>
       <c r="F191" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G191" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="G191" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="H191" s="6"/>
       <c r="I191" s="6"/>
@@ -8521,7 +8524,7 @@
       <c r="D192" s="14"/>
       <c r="E192" s="14"/>
       <c r="F192" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G192" s="7"/>
       <c r="H192" s="6"/>
@@ -8555,10 +8558,10 @@
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
       <c r="F193" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G193" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="G193" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="H193" s="6"/>
       <c r="I193" s="6"/>
@@ -8591,10 +8594,10 @@
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
       <c r="F194" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G194" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H194" s="6"/>
       <c r="I194" s="6"/>
@@ -8625,7 +8628,7 @@
         <v>51</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C195" s="13"/>
       <c r="D195" s="13" t="s">
@@ -8635,10 +8638,10 @@
         <v>55</v>
       </c>
       <c r="F195" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G195" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G195" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H195" s="6"/>
       <c r="I195" s="6"/>
@@ -8671,10 +8674,10 @@
       <c r="D196" s="14"/>
       <c r="E196" s="14"/>
       <c r="F196" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G196" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G196" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H196" s="6"/>
       <c r="I196" s="6"/>
@@ -8707,10 +8710,10 @@
       <c r="D197" s="14"/>
       <c r="E197" s="14"/>
       <c r="F197" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G197" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="G197" s="7" t="s">
-        <v>226</v>
       </c>
       <c r="H197" s="6"/>
       <c r="I197" s="6"/>
@@ -8743,10 +8746,10 @@
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="F198" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G198" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="G198" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="H198" s="6"/>
       <c r="I198" s="6"/>
@@ -8777,7 +8780,7 @@
         <v>52</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C199" s="13"/>
       <c r="D199" s="13" t="s">
@@ -8787,10 +8790,10 @@
         <v>55</v>
       </c>
       <c r="F199" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G199" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G199" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H199" s="6"/>
       <c r="I199" s="6"/>
@@ -8823,10 +8826,10 @@
       <c r="D200" s="14"/>
       <c r="E200" s="14"/>
       <c r="F200" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G200" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G200" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H200" s="6"/>
       <c r="I200" s="6"/>
@@ -8859,10 +8862,10 @@
       <c r="D201" s="14"/>
       <c r="E201" s="14"/>
       <c r="F201" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G201" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="G201" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="H201" s="6"/>
       <c r="I201" s="6"/>
@@ -8895,10 +8898,10 @@
       <c r="D202" s="14"/>
       <c r="E202" s="14"/>
       <c r="F202" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G202" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H202" s="6"/>
       <c r="I202" s="6"/>
@@ -8931,10 +8934,10 @@
       <c r="D203" s="14"/>
       <c r="E203" s="14"/>
       <c r="F203" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G203" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G203" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="H203" s="6"/>
       <c r="I203" s="6"/>
@@ -8967,10 +8970,10 @@
       <c r="D204" s="14"/>
       <c r="E204" s="14"/>
       <c r="F204" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G204" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="G204" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="H204" s="6"/>
       <c r="I204" s="6"/>
@@ -9003,10 +9006,10 @@
       <c r="D205" s="14"/>
       <c r="E205" s="14"/>
       <c r="F205" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G205" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="G205" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="H205" s="6"/>
       <c r="I205" s="6"/>
@@ -9039,7 +9042,7 @@
       <c r="D206" s="14"/>
       <c r="E206" s="14"/>
       <c r="F206" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G206" s="12"/>
       <c r="H206" s="6"/>
@@ -9073,10 +9076,10 @@
       <c r="D207" s="15"/>
       <c r="E207" s="15"/>
       <c r="F207" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H207" s="6"/>
       <c r="I207" s="6"/>
@@ -9107,7 +9110,7 @@
         <v>53</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C208" s="13"/>
       <c r="D208" s="13" t="s">
@@ -9117,10 +9120,10 @@
         <v>55</v>
       </c>
       <c r="F208" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G208" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G208" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H208" s="6"/>
       <c r="I208" s="6"/>
@@ -9153,10 +9156,10 @@
       <c r="D209" s="14"/>
       <c r="E209" s="14"/>
       <c r="F209" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G209" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G209" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H209" s="6"/>
       <c r="I209" s="6"/>
@@ -9189,10 +9192,10 @@
       <c r="D210" s="14"/>
       <c r="E210" s="14"/>
       <c r="F210" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G210" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="G210" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="H210" s="6"/>
       <c r="I210" s="6"/>
@@ -9225,10 +9228,10 @@
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
       <c r="F211" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H211" s="6"/>
       <c r="I211" s="6"/>
@@ -9261,7 +9264,7 @@
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
       <c r="F212" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G212" s="7"/>
       <c r="H212" s="6"/>
@@ -9295,10 +9298,10 @@
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
       <c r="F213" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G213" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="G213" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="H213" s="6"/>
       <c r="I213" s="6"/>
@@ -9331,10 +9334,10 @@
       <c r="D214" s="14"/>
       <c r="E214" s="14"/>
       <c r="F214" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G214" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="G214" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="H214" s="6"/>
       <c r="I214" s="6"/>
@@ -9367,7 +9370,7 @@
       <c r="D215" s="14"/>
       <c r="E215" s="14"/>
       <c r="F215" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G215" s="12"/>
       <c r="H215" s="6"/>
@@ -9401,10 +9404,10 @@
       <c r="D216" s="15"/>
       <c r="E216" s="15"/>
       <c r="F216" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G216" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H216" s="6"/>
       <c r="I216" s="6"/>
@@ -9435,7 +9438,7 @@
         <v>54</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C217" s="13"/>
       <c r="D217" s="13" t="s">
@@ -9445,10 +9448,10 @@
         <v>55</v>
       </c>
       <c r="F217" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G217" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G217" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H217" s="6"/>
       <c r="I217" s="6"/>
@@ -9481,10 +9484,10 @@
       <c r="D218" s="14"/>
       <c r="E218" s="14"/>
       <c r="F218" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G218" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G218" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H218" s="6"/>
       <c r="I218" s="6"/>
@@ -9517,10 +9520,10 @@
       <c r="D219" s="14"/>
       <c r="E219" s="14"/>
       <c r="F219" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G219" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="G219" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="H219" s="6"/>
       <c r="I219" s="6"/>
@@ -9553,10 +9556,10 @@
       <c r="D220" s="14"/>
       <c r="E220" s="14"/>
       <c r="F220" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G220" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H220" s="6"/>
       <c r="I220" s="6"/>
@@ -9589,10 +9592,10 @@
       <c r="D221" s="14"/>
       <c r="E221" s="14"/>
       <c r="F221" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G221" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G221" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="H221" s="6"/>
       <c r="I221" s="6"/>
@@ -9625,7 +9628,7 @@
       <c r="D222" s="14"/>
       <c r="E222" s="14"/>
       <c r="F222" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G222" s="7"/>
       <c r="H222" s="6"/>
@@ -9659,10 +9662,10 @@
       <c r="D223" s="14"/>
       <c r="E223" s="14"/>
       <c r="F223" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G223" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="G223" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="H223" s="6"/>
       <c r="I223" s="6"/>
@@ -9695,7 +9698,7 @@
       <c r="D224" s="14"/>
       <c r="E224" s="14"/>
       <c r="F224" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G224" s="12"/>
       <c r="H224" s="6"/>
@@ -9729,10 +9732,10 @@
       <c r="D225" s="15"/>
       <c r="E225" s="15"/>
       <c r="F225" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H225" s="6"/>
       <c r="I225" s="6"/>
@@ -9763,7 +9766,7 @@
         <v>55</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C226" s="13"/>
       <c r="D226" s="13" t="s">
@@ -9773,10 +9776,10 @@
         <v>55</v>
       </c>
       <c r="F226" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G226" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G226" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H226" s="6"/>
       <c r="I226" s="6"/>
@@ -9809,10 +9812,10 @@
       <c r="D227" s="14"/>
       <c r="E227" s="14"/>
       <c r="F227" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G227" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G227" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H227" s="6"/>
       <c r="I227" s="6"/>
@@ -9845,10 +9848,10 @@
       <c r="D228" s="14"/>
       <c r="E228" s="14"/>
       <c r="F228" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G228" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="G228" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="H228" s="6"/>
       <c r="I228" s="6"/>
@@ -9881,7 +9884,7 @@
       <c r="D229" s="14"/>
       <c r="E229" s="14"/>
       <c r="F229" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G229" s="7"/>
       <c r="H229" s="6"/>
@@ -9915,10 +9918,10 @@
       <c r="D230" s="14"/>
       <c r="E230" s="14"/>
       <c r="F230" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G230" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G230" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="H230" s="6"/>
       <c r="I230" s="6"/>
@@ -9951,10 +9954,10 @@
       <c r="D231" s="14"/>
       <c r="E231" s="14"/>
       <c r="F231" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G231" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="G231" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="H231" s="6"/>
       <c r="I231" s="6"/>
@@ -9987,10 +9990,10 @@
       <c r="D232" s="14"/>
       <c r="E232" s="14"/>
       <c r="F232" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G232" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="G232" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="H232" s="6"/>
       <c r="I232" s="6"/>
@@ -10023,7 +10026,7 @@
       <c r="D233" s="14"/>
       <c r="E233" s="14"/>
       <c r="F233" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G233" s="12"/>
       <c r="H233" s="6"/>
@@ -10057,10 +10060,10 @@
       <c r="D234" s="15"/>
       <c r="E234" s="15"/>
       <c r="F234" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G234" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H234" s="6"/>
       <c r="I234" s="6"/>
@@ -10091,7 +10094,7 @@
         <v>56</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C235" s="13"/>
       <c r="D235" s="13" t="s">
@@ -10101,10 +10104,10 @@
         <v>55</v>
       </c>
       <c r="F235" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G235" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G235" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H235" s="6"/>
       <c r="I235" s="6"/>
@@ -10137,10 +10140,10 @@
       <c r="D236" s="14"/>
       <c r="E236" s="14"/>
       <c r="F236" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G236" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="G236" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="H236" s="6"/>
       <c r="I236" s="6"/>
@@ -10173,10 +10176,10 @@
       <c r="D237" s="14"/>
       <c r="E237" s="14"/>
       <c r="F237" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G237" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G237" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H237" s="6"/>
       <c r="I237" s="6"/>
@@ -10209,10 +10212,10 @@
       <c r="D238" s="14"/>
       <c r="E238" s="14"/>
       <c r="F238" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G238" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="G238" s="7" t="s">
-        <v>231</v>
       </c>
       <c r="H238" s="6"/>
       <c r="I238" s="6"/>
@@ -10245,10 +10248,10 @@
       <c r="D239" s="14"/>
       <c r="E239" s="14"/>
       <c r="F239" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G239" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H239" s="6"/>
       <c r="I239" s="6"/>
@@ -10281,10 +10284,10 @@
       <c r="D240" s="14"/>
       <c r="E240" s="14"/>
       <c r="F240" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G240" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G240" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="H240" s="6"/>
       <c r="I240" s="6"/>
@@ -10317,10 +10320,10 @@
       <c r="D241" s="14"/>
       <c r="E241" s="14"/>
       <c r="F241" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G241" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="G241" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="H241" s="6"/>
       <c r="I241" s="6"/>
@@ -10353,10 +10356,10 @@
       <c r="D242" s="14"/>
       <c r="E242" s="14"/>
       <c r="F242" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G242" s="7" t="s">
         <v>237</v>
-      </c>
-      <c r="G242" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="H242" s="6"/>
       <c r="I242" s="6"/>
@@ -10389,7 +10392,7 @@
       <c r="D243" s="14"/>
       <c r="E243" s="14"/>
       <c r="F243" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G243" s="12"/>
       <c r="H243" s="6"/>
@@ -10423,10 +10426,10 @@
       <c r="D244" s="14"/>
       <c r="E244" s="14"/>
       <c r="F244" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G244" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H244" s="6"/>
       <c r="I244" s="6"/>
@@ -10459,10 +10462,10 @@
       <c r="D245" s="14"/>
       <c r="E245" s="14"/>
       <c r="F245" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G245" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H245" s="6"/>
       <c r="I245" s="6"/>
@@ -10495,10 +10498,10 @@
       <c r="D246" s="14"/>
       <c r="E246" s="14"/>
       <c r="F246" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G246" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H246" s="6"/>
       <c r="I246" s="6"/>
@@ -10531,10 +10534,10 @@
       <c r="D247" s="14"/>
       <c r="E247" s="14"/>
       <c r="F247" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="G247" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="G247" s="7" t="s">
-        <v>253</v>
       </c>
       <c r="H247" s="6"/>
       <c r="I247" s="6"/>
@@ -10567,10 +10570,10 @@
       <c r="D248" s="15"/>
       <c r="E248" s="15"/>
       <c r="F248" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G248" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="G248" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="H248" s="6"/>
       <c r="I248" s="6"/>
@@ -35878,60 +35881,186 @@
     </row>
   </sheetData>
   <mergeCells count="280">
-    <mergeCell ref="A66:A71"/>
-    <mergeCell ref="D106:D111"/>
-    <mergeCell ref="C106:C111"/>
-    <mergeCell ref="B217:B225"/>
-    <mergeCell ref="B226:B234"/>
-    <mergeCell ref="B208:B216"/>
-    <mergeCell ref="C208:C216"/>
-    <mergeCell ref="D208:D216"/>
-    <mergeCell ref="E208:E216"/>
-    <mergeCell ref="C217:C225"/>
-    <mergeCell ref="D217:D225"/>
-    <mergeCell ref="E217:E225"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D72:D77"/>
+    <mergeCell ref="E72:E77"/>
+    <mergeCell ref="C78:C83"/>
+    <mergeCell ref="B78:B83"/>
+    <mergeCell ref="D78:D83"/>
+    <mergeCell ref="E78:E83"/>
+    <mergeCell ref="D84:D89"/>
+    <mergeCell ref="C84:C89"/>
+    <mergeCell ref="E90:E93"/>
+    <mergeCell ref="E84:E89"/>
+    <mergeCell ref="D90:D93"/>
+    <mergeCell ref="C94:C99"/>
+    <mergeCell ref="D94:D99"/>
+    <mergeCell ref="E94:E99"/>
+    <mergeCell ref="B84:B89"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="E47:E49"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="D66:D71"/>
+    <mergeCell ref="E66:E71"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B94:B99"/>
+    <mergeCell ref="A94:A99"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A78:A83"/>
+    <mergeCell ref="A72:A77"/>
+    <mergeCell ref="A84:A89"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B71"/>
+    <mergeCell ref="C66:C71"/>
+    <mergeCell ref="B72:B77"/>
+    <mergeCell ref="C72:C77"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="E142:E143"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="E144:E145"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="E161:E166"/>
+    <mergeCell ref="D148:D150"/>
+    <mergeCell ref="E148:E150"/>
+    <mergeCell ref="D151:D153"/>
+    <mergeCell ref="E151:E153"/>
+    <mergeCell ref="D154:D157"/>
+    <mergeCell ref="E154:E157"/>
+    <mergeCell ref="E158:E160"/>
+    <mergeCell ref="A154:A157"/>
+    <mergeCell ref="A158:A160"/>
+    <mergeCell ref="B158:B160"/>
+    <mergeCell ref="C158:C160"/>
+    <mergeCell ref="A161:A166"/>
+    <mergeCell ref="B161:B166"/>
+    <mergeCell ref="C161:C166"/>
+    <mergeCell ref="B154:B157"/>
+    <mergeCell ref="E134:E140"/>
+    <mergeCell ref="A134:A140"/>
+    <mergeCell ref="B148:B150"/>
+    <mergeCell ref="C148:C150"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="B151:B153"/>
+    <mergeCell ref="C151:C153"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="D146:D147"/>
+    <mergeCell ref="E146:E147"/>
+    <mergeCell ref="A148:A150"/>
+    <mergeCell ref="E100:E105"/>
+    <mergeCell ref="C100:C105"/>
+    <mergeCell ref="A100:A105"/>
+    <mergeCell ref="E106:E111"/>
+    <mergeCell ref="A106:A111"/>
+    <mergeCell ref="C154:C157"/>
+    <mergeCell ref="B123:B126"/>
+    <mergeCell ref="E123:E126"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="D144:D145"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="B112:B114"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="B115:B118"/>
+    <mergeCell ref="B119:B122"/>
+    <mergeCell ref="D115:D118"/>
+    <mergeCell ref="C115:C118"/>
+    <mergeCell ref="E115:E118"/>
+    <mergeCell ref="E119:E122"/>
+    <mergeCell ref="D119:D122"/>
+    <mergeCell ref="C119:C122"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="E127:E133"/>
+    <mergeCell ref="D127:D133"/>
+    <mergeCell ref="B188:B194"/>
+    <mergeCell ref="C188:C194"/>
+    <mergeCell ref="D188:D194"/>
+    <mergeCell ref="A181:A187"/>
+    <mergeCell ref="A188:A194"/>
+    <mergeCell ref="B167:B173"/>
+    <mergeCell ref="C167:C173"/>
+    <mergeCell ref="D167:D173"/>
+    <mergeCell ref="B100:B105"/>
+    <mergeCell ref="B106:B111"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="D100:D105"/>
+    <mergeCell ref="C127:C133"/>
+    <mergeCell ref="B127:B133"/>
+    <mergeCell ref="D123:D126"/>
+    <mergeCell ref="C123:C126"/>
+    <mergeCell ref="A112:A114"/>
+    <mergeCell ref="B134:B140"/>
+    <mergeCell ref="D134:D140"/>
+    <mergeCell ref="C134:C140"/>
+    <mergeCell ref="D158:D160"/>
+    <mergeCell ref="D161:D166"/>
+    <mergeCell ref="A127:A133"/>
+    <mergeCell ref="E23:E27"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="A235:A248"/>
+    <mergeCell ref="A226:A234"/>
+    <mergeCell ref="A217:A225"/>
+    <mergeCell ref="B235:B248"/>
+    <mergeCell ref="C235:C248"/>
+    <mergeCell ref="D235:D248"/>
+    <mergeCell ref="E235:E248"/>
+    <mergeCell ref="C226:C234"/>
+    <mergeCell ref="D226:D234"/>
+    <mergeCell ref="E226:E234"/>
+    <mergeCell ref="E167:E173"/>
+    <mergeCell ref="A195:A198"/>
+    <mergeCell ref="E195:E198"/>
+    <mergeCell ref="E188:E194"/>
+    <mergeCell ref="A167:A173"/>
+    <mergeCell ref="A174:A180"/>
+    <mergeCell ref="A208:A216"/>
+    <mergeCell ref="B174:B180"/>
+    <mergeCell ref="C174:C180"/>
+    <mergeCell ref="D174:D180"/>
+    <mergeCell ref="E174:E180"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -35956,30 +36085,70 @@
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="C23:C27"/>
     <mergeCell ref="D23:D27"/>
-    <mergeCell ref="E23:E27"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A235:A248"/>
-    <mergeCell ref="A226:A234"/>
-    <mergeCell ref="A217:A225"/>
-    <mergeCell ref="B235:B248"/>
-    <mergeCell ref="C235:C248"/>
-    <mergeCell ref="D235:D248"/>
-    <mergeCell ref="E235:E248"/>
-    <mergeCell ref="C226:C234"/>
-    <mergeCell ref="D226:D234"/>
-    <mergeCell ref="E226:E234"/>
-    <mergeCell ref="E167:E173"/>
-    <mergeCell ref="A195:A198"/>
-    <mergeCell ref="E195:E198"/>
-    <mergeCell ref="E188:E194"/>
-    <mergeCell ref="A167:A173"/>
-    <mergeCell ref="A174:A180"/>
-    <mergeCell ref="A208:A216"/>
-    <mergeCell ref="B174:B180"/>
-    <mergeCell ref="C174:C180"/>
-    <mergeCell ref="D174:D180"/>
-    <mergeCell ref="E174:E180"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="D106:D111"/>
+    <mergeCell ref="C106:C111"/>
+    <mergeCell ref="B217:B225"/>
+    <mergeCell ref="B226:B234"/>
+    <mergeCell ref="B208:B216"/>
+    <mergeCell ref="C208:C216"/>
+    <mergeCell ref="D208:D216"/>
+    <mergeCell ref="E208:E216"/>
+    <mergeCell ref="C217:C225"/>
+    <mergeCell ref="D217:D225"/>
+    <mergeCell ref="E217:E225"/>
     <mergeCell ref="B181:B187"/>
     <mergeCell ref="C181:C187"/>
     <mergeCell ref="D181:D187"/>
@@ -35992,172 +36161,6 @@
     <mergeCell ref="D199:D207"/>
     <mergeCell ref="E199:E207"/>
     <mergeCell ref="B195:B198"/>
-    <mergeCell ref="B188:B194"/>
-    <mergeCell ref="C188:C194"/>
-    <mergeCell ref="D188:D194"/>
-    <mergeCell ref="A181:A187"/>
-    <mergeCell ref="A188:A194"/>
-    <mergeCell ref="B167:B173"/>
-    <mergeCell ref="C167:C173"/>
-    <mergeCell ref="D167:D173"/>
-    <mergeCell ref="B100:B105"/>
-    <mergeCell ref="B106:B111"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A119:A122"/>
-    <mergeCell ref="D100:D105"/>
-    <mergeCell ref="E100:E105"/>
-    <mergeCell ref="C100:C105"/>
-    <mergeCell ref="A100:A105"/>
-    <mergeCell ref="E106:E111"/>
-    <mergeCell ref="A106:A111"/>
-    <mergeCell ref="C154:C157"/>
-    <mergeCell ref="B123:B126"/>
-    <mergeCell ref="E123:E126"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="D144:D145"/>
-    <mergeCell ref="E112:E114"/>
-    <mergeCell ref="B112:B114"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="B115:B118"/>
-    <mergeCell ref="B119:B122"/>
-    <mergeCell ref="D115:D118"/>
-    <mergeCell ref="C115:C118"/>
-    <mergeCell ref="E115:E118"/>
-    <mergeCell ref="E119:E122"/>
-    <mergeCell ref="D119:D122"/>
-    <mergeCell ref="C119:C122"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="E127:E133"/>
-    <mergeCell ref="D127:D133"/>
-    <mergeCell ref="C127:C133"/>
-    <mergeCell ref="B127:B133"/>
-    <mergeCell ref="D123:D126"/>
-    <mergeCell ref="C123:C126"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="B134:B140"/>
-    <mergeCell ref="D134:D140"/>
-    <mergeCell ref="C134:C140"/>
-    <mergeCell ref="E134:E140"/>
-    <mergeCell ref="A134:A140"/>
-    <mergeCell ref="B148:B150"/>
-    <mergeCell ref="C148:C150"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="B151:B153"/>
-    <mergeCell ref="C151:C153"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="D146:D147"/>
-    <mergeCell ref="E146:E147"/>
-    <mergeCell ref="A148:A150"/>
-    <mergeCell ref="D158:D160"/>
-    <mergeCell ref="D161:D166"/>
-    <mergeCell ref="E161:E166"/>
-    <mergeCell ref="D148:D150"/>
-    <mergeCell ref="E148:E150"/>
-    <mergeCell ref="D151:D153"/>
-    <mergeCell ref="E151:E153"/>
-    <mergeCell ref="D154:D157"/>
-    <mergeCell ref="E154:E157"/>
-    <mergeCell ref="E158:E160"/>
-    <mergeCell ref="A154:A157"/>
-    <mergeCell ref="A158:A160"/>
-    <mergeCell ref="B158:B160"/>
-    <mergeCell ref="C158:C160"/>
-    <mergeCell ref="A161:A166"/>
-    <mergeCell ref="B161:B166"/>
-    <mergeCell ref="C161:C166"/>
-    <mergeCell ref="B154:B157"/>
-    <mergeCell ref="A127:A133"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D142:D143"/>
-    <mergeCell ref="E142:E143"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="E144:E145"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="B94:B99"/>
-    <mergeCell ref="A94:A99"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A78:A83"/>
-    <mergeCell ref="A72:A77"/>
-    <mergeCell ref="A84:A89"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B66:B71"/>
-    <mergeCell ref="C66:C71"/>
-    <mergeCell ref="D90:D93"/>
-    <mergeCell ref="C94:C99"/>
-    <mergeCell ref="D94:D99"/>
-    <mergeCell ref="E94:E99"/>
-    <mergeCell ref="B84:B89"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="D66:D71"/>
-    <mergeCell ref="E66:E71"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="B72:B77"/>
-    <mergeCell ref="C72:C77"/>
-    <mergeCell ref="D72:D77"/>
-    <mergeCell ref="E72:E77"/>
-    <mergeCell ref="C78:C83"/>
-    <mergeCell ref="B78:B83"/>
-    <mergeCell ref="D78:D83"/>
-    <mergeCell ref="E78:E83"/>
-    <mergeCell ref="D84:D89"/>
-    <mergeCell ref="C84:C89"/>
-    <mergeCell ref="E90:E93"/>
-    <mergeCell ref="E84:E89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>